<commit_message>
psychopy-2 : multiple foods, two loops; now must do actual conditions
</commit_message>
<xml_diff>
--- a/psychopy-2/irrelevant.xlsx
+++ b/psychopy-2/irrelevant.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8360" yWindow="-17900" windowWidth="20500" windowHeight="12780" tabRatio="500"/>
+    <workbookView xWindow="8180" yWindow="640" windowWidth="20500" windowHeight="12780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,23 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>corrAns</t>
   </si>
   <si>
-    <t>Molina's Cantina</t>
-  </si>
-  <si>
-    <t>Restaurante Arroyo</t>
-  </si>
-  <si>
-    <t>mexican_food1</t>
-  </si>
-  <si>
-    <t>mexican_food2</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -48,22 +36,19 @@
     <t>right</t>
   </si>
   <si>
-    <t>restaurant</t>
-  </si>
-  <si>
-    <t>food</t>
-  </si>
-  <si>
     <t>sick</t>
   </si>
   <si>
-    <t>mexican_food3</t>
-  </si>
-  <si>
     <t>Training</t>
   </si>
   <si>
     <t xml:space="preserve"> Test</t>
+  </si>
+  <si>
+    <t>contextId</t>
+  </si>
+  <si>
+    <t>cueId</t>
   </si>
 </sst>
 </file>
@@ -134,8 +119,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -161,7 +152,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -170,6 +161,9 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -178,6 +172,9 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -510,7 +507,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -521,13 +518,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -535,120 +532,120 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" t="s">
+      <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>12</v>
+      <c r="A10" s="1">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" t="s">
+      <c r="A11">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
-        <v>12</v>
+      <c r="B11">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3 context roles! woohoo. Now time to randomize 'em also don't forget to randomize the loops too
</commit_message>
<xml_diff>
--- a/psychopy-2/irrelevant.xlsx
+++ b/psychopy-2/irrelevant.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>corrAns</t>
   </si>
@@ -507,7 +507,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -609,12 +609,6 @@
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
@@ -622,12 +616,6 @@
       </c>
       <c r="B9">
         <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4">

</xml_diff>